<commit_message>
[update] result for VGG10->Fashion, CIFAR10; LeNet9->Fashion
</commit_message>
<xml_diff>
--- a/results/VGG10 results.xlsx
+++ b/results/VGG10 results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyCourse(5 delayed 1)\erasure code\SUSTech-Coded-Computation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECF123E-E8E6-4022-A8B1-47950C17C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F91411-9700-4E2A-B4B9-8B1ACB9AC577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14784" yWindow="804" windowWidth="10296" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="228" yWindow="372" windowWidth="10296" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,6 +294,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -306,8 +309,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="D55" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -601,19 +607,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -651,13 +657,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
         <v>3</v>
       </c>
       <c r="D3" s="2">
@@ -666,7 +672,7 @@
       <c r="E3" s="2">
         <v>0.99350000000000005</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="3">
@@ -689,16 +695,16 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E4" s="2">
         <v>0.99350000000000005</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="4">
         <v>1</v>
       </c>
@@ -719,16 +725,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E5" s="2">
         <v>0.99350000000000005</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="3">
         <v>2</v>
       </c>
@@ -749,16 +755,16 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E6" s="2">
         <v>0.99350000000000005</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="3">
         <v>3</v>
       </c>
@@ -779,16 +785,16 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E7" s="2">
         <v>0.99050000000000005</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="3">
@@ -811,16 +817,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E8" s="2">
         <v>0.99050000000000005</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="6">
         <v>1</v>
       </c>
@@ -841,16 +847,16 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E9" s="2">
         <v>0.99050000000000005</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="3">
         <v>2</v>
       </c>
@@ -871,16 +877,16 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E10" s="2">
         <v>0.99050000000000005</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="3">
         <v>3</v>
       </c>
@@ -936,13 +942,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="13">
         <v>2</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="13">
         <v>6</v>
       </c>
       <c r="D12" s="2">
@@ -951,7 +957,7 @@
       <c r="E12" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="3">
@@ -974,16 +980,16 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E13" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="4">
         <v>1</v>
       </c>
@@ -1004,16 +1010,16 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E14" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="4">
         <v>2</v>
       </c>
@@ -1034,16 +1040,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E15" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="3">
         <v>3</v>
       </c>
@@ -1064,16 +1070,16 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E16" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="3">
         <v>4</v>
       </c>
@@ -1094,16 +1100,16 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E17" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="3">
         <v>5</v>
       </c>
@@ -1124,16 +1130,16 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="2">
         <v>0.99399999999999999</v>
       </c>
       <c r="E18" s="2">
         <v>0.9929</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="3">
         <v>6</v>
       </c>
@@ -1154,16 +1160,16 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E19" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="3">
@@ -1186,16 +1192,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E20" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="6">
         <v>1</v>
       </c>
@@ -1216,16 +1222,16 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E21" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="6">
         <v>2</v>
       </c>
@@ -1246,16 +1252,16 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E22" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="3">
         <v>3</v>
       </c>
@@ -1276,16 +1282,16 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E23" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="3">
         <v>4</v>
       </c>
@@ -1306,16 +1312,16 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E24" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="3">
         <v>5</v>
       </c>
@@ -1336,16 +1342,16 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="2">
         <v>0.99139999999999995</v>
       </c>
       <c r="E25" s="2">
         <v>0.9899</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="3">
         <v>6</v>
       </c>
@@ -1379,19 +1385,19 @@
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1429,37 +1435,37 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="10">
         <v>2</v>
       </c>
-      <c r="B29" s="9">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9">
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" s="10">
         <v>3</v>
       </c>
       <c r="D29" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E29" s="2">
-        <v>0.95930000000000004</v>
-      </c>
-      <c r="F29" s="9" t="s">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
       </c>
       <c r="H29" s="2">
-        <v>0.95930000000000004</v>
+        <v>0.98329999999999995</v>
       </c>
       <c r="I29" s="2">
         <f>D29-H29</f>
-        <v>6.5999999999999392E-3</v>
+        <v>1.2700000000000045E-2</v>
       </c>
       <c r="J29" s="2">
         <f>H29/D29</f>
-        <v>0.99316699451288959</v>
+        <v>0.98724899598393567</v>
       </c>
       <c r="K29" s="2">
         <f>H29/E29</f>
@@ -1467,76 +1473,76 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E30" s="2">
-        <v>0.95930000000000004</v>
-      </c>
-      <c r="F30" s="10"/>
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="F30" s="11"/>
       <c r="G30" s="4">
         <v>1</v>
       </c>
       <c r="H30" s="5">
-        <v>0.90049999999999997</v>
+        <v>0.9294</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" ref="I30:I36" si="7">D30-H30</f>
-        <v>6.5400000000000014E-2</v>
+        <v>6.6599999999999993E-2</v>
       </c>
       <c r="J30" s="5">
         <f>H30/D30</f>
-        <v>0.93229112744590537</v>
+        <v>0.93313253012048192</v>
       </c>
       <c r="K30" s="5">
         <f>H30/E30</f>
-        <v>0.93870530595225676</v>
+        <v>0.94518458252822135</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E31" s="2">
-        <v>0.95930000000000004</v>
-      </c>
-      <c r="F31" s="10"/>
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="F31" s="11"/>
       <c r="G31" s="3">
         <v>2</v>
       </c>
       <c r="H31" s="2">
-        <v>0.61140000000000005</v>
+        <v>0.66910000000000003</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="7"/>
-        <v>0.35449999999999993</v>
+        <v>0.32689999999999997</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" ref="J31:J36" si="8">H31/D31</f>
-        <v>0.6329847810332333</v>
+        <v>0.67178714859437749</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" ref="K31:K36" si="9">H31/E31</f>
-        <v>0.63733972688418639</v>
+        <v>0.68046374453371306</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E32" s="2">
-        <v>0.95930000000000004</v>
-      </c>
-      <c r="F32" s="11"/>
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="F32" s="12"/>
       <c r="G32" s="3">
         <v>3</v>
       </c>
@@ -1545,43 +1551,43 @@
       </c>
       <c r="I32" s="2">
         <f t="shared" si="7"/>
-        <v>0.8659</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="8"/>
-        <v>0.10353038616834041</v>
+        <v>0.10040160642570281</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="9"/>
-        <v>0.10424267695194413</v>
+        <v>0.10169836265636124</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E33" s="2">
-        <v>0.9264</v>
-      </c>
-      <c r="F33" s="9" t="s">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G33" s="3">
         <v>0</v>
       </c>
       <c r="H33" s="2">
-        <v>0.9264</v>
+        <v>0.92889999999999995</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="7"/>
-        <v>2.3999999999999577E-3</v>
+        <v>4.2000000000000925E-3</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="8"/>
-        <v>0.99741602067183466</v>
+        <v>0.99549887471867959</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="9"/>
@@ -1589,76 +1595,76 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E34" s="2">
-        <v>0.9264</v>
-      </c>
-      <c r="F34" s="10"/>
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="F34" s="11"/>
       <c r="G34" s="6">
         <v>1</v>
       </c>
       <c r="H34" s="7">
-        <v>0.8841</v>
+        <v>0.88560000000000005</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="7"/>
-        <v>4.4699999999999962E-2</v>
+        <v>4.7499999999999987E-2</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="8"/>
-        <v>0.95187338501291996</v>
+        <v>0.94909441646125814</v>
       </c>
       <c r="K34" s="7">
         <f t="shared" si="9"/>
-        <v>0.95433937823834192</v>
+        <v>0.95338572505113583</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E35" s="2">
-        <v>0.9264</v>
-      </c>
-      <c r="F35" s="10"/>
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="F35" s="11"/>
       <c r="G35" s="3">
         <v>2</v>
       </c>
       <c r="H35" s="2">
-        <v>0.64770000000000005</v>
+        <v>0.67879999999999996</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="7"/>
-        <v>0.28109999999999991</v>
+        <v>0.25430000000000008</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="8"/>
-        <v>0.69735142118863058</v>
+        <v>0.72746758118100951</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="9"/>
-        <v>0.69915803108808294</v>
+        <v>0.73075680912907737</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E36" s="2">
-        <v>0.9264</v>
-      </c>
-      <c r="F36" s="11"/>
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="F36" s="12"/>
       <c r="G36" s="3">
         <v>3</v>
       </c>
@@ -1667,15 +1673,15 @@
       </c>
       <c r="I36" s="2">
         <f t="shared" si="7"/>
-        <v>0.82879999999999998</v>
+        <v>0.83310000000000006</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="8"/>
-        <v>0.10766580534022395</v>
+        <v>0.10716964955524595</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="9"/>
-        <v>0.1079447322970639</v>
+        <v>0.10765421466250405</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1714,37 +1720,37 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+      <c r="A38" s="13">
         <v>4</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="13">
         <v>2</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="13">
         <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E38" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F38" s="12" t="s">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F38" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="3">
         <v>0</v>
       </c>
       <c r="H38" s="2">
-        <v>0.95479999999999998</v>
+        <v>0.98250000000000004</v>
       </c>
       <c r="I38" s="2">
         <f>D38-H38</f>
-        <v>1.1099999999999999E-2</v>
+        <v>1.3499999999999956E-2</v>
       </c>
       <c r="J38" s="2">
         <f>H38/D38</f>
-        <v>0.98850812713531422</v>
+        <v>0.98644578313253017</v>
       </c>
       <c r="K38" s="2">
         <f>H38/E38</f>
@@ -1752,166 +1758,166 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E39" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F39" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F39" s="13"/>
       <c r="G39" s="4">
         <v>1</v>
       </c>
-      <c r="H39" s="5">
-        <v>0.94140000000000001</v>
+      <c r="H39" s="14">
+        <v>0.96989999999999998</v>
       </c>
       <c r="I39" s="5">
-        <f>D38-H39</f>
-        <v>2.4499999999999966E-2</v>
+        <f>D38-H40</f>
+        <v>4.7300000000000009E-2</v>
       </c>
       <c r="J39" s="5">
-        <f>H39/D39</f>
-        <v>0.97463505538875661</v>
+        <f>H40/D39</f>
+        <v>0.95251004016064256</v>
       </c>
       <c r="K39" s="5">
-        <f>H39/E39</f>
-        <v>0.98596564725596991</v>
+        <f>H40/E39</f>
+        <v>0.96559796437659029</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E40" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F40" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F40" s="13"/>
       <c r="G40" s="4">
         <v>2</v>
       </c>
       <c r="H40" s="5">
-        <v>0.92210000000000003</v>
+        <v>0.94869999999999999</v>
       </c>
       <c r="I40" s="5">
-        <f>D38-H40</f>
-        <v>4.379999999999995E-2</v>
+        <f>D38-H41</f>
+        <v>8.2699999999999996E-2</v>
       </c>
       <c r="J40" s="5">
-        <f>H40/D40</f>
-        <v>0.9546536908582669</v>
+        <f>H41/D40</f>
+        <v>0.91696787148594383</v>
       </c>
       <c r="K40" s="5">
-        <f>H40/E40</f>
-        <v>0.96575198994553835</v>
+        <f>H41/E40</f>
+        <v>0.92956743002544528</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E41" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F41" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F41" s="13"/>
       <c r="G41" s="3">
         <v>3</v>
       </c>
-      <c r="H41" s="2">
-        <v>0.88429999999999997</v>
+      <c r="H41" s="15">
+        <v>0.9133</v>
       </c>
       <c r="I41" s="2">
-        <f>D41-H41</f>
-        <v>8.1600000000000006E-2</v>
+        <f>D41-H42</f>
+        <v>0.16310000000000002</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" ref="J41:J51" si="10">H41/D41</f>
-        <v>0.91551920488663419</v>
+        <f>H42/D41</f>
+        <v>0.83624497991967872</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" ref="K41:K51" si="11">H41/E41</f>
-        <v>0.926162547130289</v>
+        <f>H42/E41</f>
+        <v>0.84773536895674295</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E42" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F42" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F42" s="13"/>
       <c r="G42" s="3">
         <v>4</v>
       </c>
       <c r="H42" s="2">
-        <v>0.79779999999999995</v>
+        <v>0.83289999999999997</v>
       </c>
       <c r="I42" s="2">
-        <f>D42-H42</f>
-        <v>0.16810000000000003</v>
+        <f>D42-H43</f>
+        <v>0.39070000000000005</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="10"/>
-        <v>0.82596542085101976</v>
+        <f>H43/D42</f>
+        <v>0.6077309236947791</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="11"/>
-        <v>0.83556765814830325</v>
+        <f>H43/E42</f>
+        <v>0.61608142493638673</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E43" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F43" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F43" s="13"/>
       <c r="G43" s="3">
         <v>5</v>
       </c>
       <c r="H43" s="2">
-        <v>0.57540000000000002</v>
+        <v>0.60529999999999995</v>
       </c>
       <c r="I43" s="2">
-        <f>D42-H43</f>
-        <v>0.39049999999999996</v>
+        <f>D43-H44</f>
+        <v>0.89600000000000002</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="10"/>
-        <v>0.59571384201263078</v>
+        <f>H44/D43</f>
+        <v>0.10040160642570281</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="11"/>
-        <v>0.6026392961876833</v>
+        <f>H44/E43</f>
+        <v>0.10178117048346057</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="2">
-        <v>0.96589999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="E44" s="2">
-        <v>0.95479999999999998</v>
-      </c>
-      <c r="F44" s="12"/>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F44" s="13"/>
       <c r="G44" s="3">
         <v>6</v>
       </c>
@@ -1920,43 +1926,43 @@
       </c>
       <c r="I44" s="2">
         <f>D42-H44</f>
-        <v>0.8659</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="10"/>
-        <v>0.10353038616834041</v>
+        <f t="shared" ref="J41:J51" si="10">H44/D44</f>
+        <v>0.10040160642570281</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="11"/>
-        <v>0.10473397570171765</v>
+        <f t="shared" ref="K41:K51" si="11">H44/E44</f>
+        <v>0.10178117048346057</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E45" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F45" s="12" t="s">
+        <v>0.9304</v>
+      </c>
+      <c r="F45" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45" s="2">
-        <v>0.92600000000000005</v>
+        <v>0.9304</v>
       </c>
       <c r="I45" s="2">
         <f>D45-H45</f>
-        <v>2.7999999999999137E-3</v>
+        <v>2.7000000000000357E-3</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="10"/>
-        <v>0.99698535745047379</v>
+        <v>0.99710641946200829</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="11"/>
@@ -1964,166 +1970,166 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E46" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F46" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F46" s="13"/>
       <c r="G46" s="6">
         <v>1</v>
       </c>
       <c r="H46" s="7">
-        <v>0.9133</v>
+        <v>0.92420000000000002</v>
       </c>
       <c r="I46" s="7">
         <f>D46-H46</f>
-        <v>1.5499999999999958E-2</v>
+        <v>8.900000000000019E-3</v>
       </c>
       <c r="J46" s="7">
         <f t="shared" si="10"/>
-        <v>0.98331180017226538</v>
+        <v>0.9904619011895831</v>
       </c>
       <c r="K46" s="7">
         <f t="shared" si="11"/>
-        <v>0.98628509719222457</v>
+        <v>0.99333619948409291</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E47" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F47" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F47" s="13"/>
       <c r="G47" s="6">
         <v>2</v>
       </c>
       <c r="H47" s="7">
-        <v>0.90190000000000003</v>
+        <v>0.90549999999999997</v>
       </c>
       <c r="I47" s="7">
         <f>D46-H47</f>
-        <v>2.6899999999999924E-2</v>
+        <v>2.7600000000000069E-2</v>
       </c>
       <c r="J47" s="7">
         <f t="shared" si="10"/>
-        <v>0.97103789836347987</v>
+        <v>0.97042117672275208</v>
       </c>
       <c r="K47" s="7">
         <f t="shared" si="11"/>
-        <v>0.97397408207343417</v>
+        <v>0.97323731728288909</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E48" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F48" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F48" s="13"/>
       <c r="G48" s="3">
         <v>3</v>
       </c>
       <c r="H48" s="2">
-        <v>0.8579</v>
+        <v>0.87570000000000003</v>
       </c>
       <c r="I48" s="2">
         <f>D46-H48</f>
-        <v>7.0899999999999963E-2</v>
+        <v>5.7400000000000007E-2</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="10"/>
-        <v>0.9236649440137813</v>
+        <v>0.93848462115528886</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="11"/>
-        <v>0.92645788336933044</v>
+        <v>0.94120808254514188</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E49" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F49" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F49" s="13"/>
       <c r="G49" s="3">
         <v>4</v>
       </c>
       <c r="H49" s="2">
-        <v>0.79469999999999996</v>
+        <v>0.80130000000000001</v>
       </c>
       <c r="I49" s="2">
         <f>D49-H49</f>
-        <v>0.1341</v>
+        <v>0.13180000000000003</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="10"/>
-        <v>0.85562015503875966</v>
+        <v>0.85875040188618579</v>
       </c>
       <c r="K49" s="2">
         <f t="shared" si="11"/>
-        <v>0.85820734341252691</v>
+        <v>0.86124247635425621</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
       <c r="D50" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E50" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F50" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F50" s="13"/>
       <c r="G50" s="3">
         <v>5</v>
       </c>
       <c r="H50" s="2">
-        <v>0.57609999999999995</v>
+        <v>0.59940000000000004</v>
       </c>
       <c r="I50" s="2">
         <f>D50-H50</f>
-        <v>0.35270000000000001</v>
+        <v>0.3337</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="10"/>
-        <v>0.62026270456503008</v>
+        <v>0.64237487943414429</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="11"/>
-        <v>0.62213822894168458</v>
+        <v>0.64423903697334484</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="2">
-        <v>0.92879999999999996</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="E51" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="F51" s="12"/>
+        <v>0.9304</v>
+      </c>
+      <c r="F51" s="13"/>
       <c r="G51" s="3">
         <v>6</v>
       </c>
@@ -2132,15 +2138,15 @@
       </c>
       <c r="I51" s="2">
         <f>D50-H51</f>
-        <v>0.82879999999999998</v>
+        <v>0.83310000000000006</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="10"/>
-        <v>0.10766580534022395</v>
+        <v>0.10716964955524595</v>
       </c>
       <c r="K51" s="2">
         <f t="shared" si="11"/>
-        <v>0.10799136069114471</v>
+        <v>0.10748065348237318</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2157,19 +2163,19 @@
       <c r="K52" s="8"/>
     </row>
     <row r="53" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -2207,205 +2213,253 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="10">
         <v>2</v>
       </c>
-      <c r="B55" s="9">
-        <v>1</v>
-      </c>
-      <c r="C55" s="9">
+      <c r="B55" s="10">
+        <v>1</v>
+      </c>
+      <c r="C55" s="10">
         <v>3</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="9" t="s">
+      <c r="D55" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="F55" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G55" s="3">
         <v>0</v>
       </c>
-      <c r="H55" s="2"/>
+      <c r="H55" s="2">
+        <v>0.95030000000000003</v>
+      </c>
       <c r="I55" s="2">
         <f t="shared" ref="I55:I62" si="12">D55-H55</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="3" t="e">
+        <v>3.9799999999999947E-2</v>
+      </c>
+      <c r="J55" s="2">
         <f>H55/D55</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K55" s="3" t="e">
+        <v>0.95980204019795989</v>
+      </c>
+      <c r="K55" s="2">
         <f>H55/E55</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="10"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="F56" s="11"/>
       <c r="G56" s="4">
         <v>1</v>
       </c>
-      <c r="H56" s="5"/>
+      <c r="H56" s="5">
+        <v>0.85229999999999995</v>
+      </c>
       <c r="I56" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="4" t="e">
+        <v>0.13780000000000003</v>
+      </c>
+      <c r="J56" s="5">
         <f t="shared" ref="J56:J62" si="13">H56/D56</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K56" s="4" t="e">
+        <v>0.86082213917786077</v>
+      </c>
+      <c r="K56" s="5">
         <f t="shared" ref="K56:K62" si="14">H56/E56</f>
-        <v>#DIV/0!</v>
+        <v>0.89687467115647679</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="10"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="F57" s="11"/>
       <c r="G57" s="3">
         <v>2</v>
       </c>
-      <c r="H57" s="2"/>
+      <c r="H57" s="2">
+        <v>0.53</v>
+      </c>
       <c r="I57" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="3" t="e">
+        <v>0.46009999999999995</v>
+      </c>
+      <c r="J57" s="2">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="3" t="e">
+        <v>0.53529946470053535</v>
+      </c>
+      <c r="K57" s="2">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>0.55771861517415555</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="11"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="F58" s="12"/>
       <c r="G58" s="3">
         <v>3</v>
       </c>
-      <c r="H58" s="2"/>
+      <c r="H58" s="2">
+        <v>0.1</v>
+      </c>
       <c r="I58" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J58" s="3" t="e">
+        <v>0.8901</v>
+      </c>
+      <c r="J58" s="2">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K58" s="3" t="e">
+        <v>0.10099989900010101</v>
+      </c>
+      <c r="K58" s="2">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>0.10522992739135011</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="9" t="s">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G59" s="3">
         <v>0</v>
       </c>
-      <c r="H59" s="2"/>
+      <c r="H59" s="2">
+        <v>0.83299999999999996</v>
+      </c>
       <c r="I59" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="3" t="e">
+        <v>1.430000000000009E-2</v>
+      </c>
+      <c r="J59" s="2">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K59" s="3" t="e">
+        <v>0.98312286085211842</v>
+      </c>
+      <c r="K59" s="2">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="10"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F60" s="11"/>
       <c r="G60" s="6">
         <v>1</v>
       </c>
-      <c r="H60" s="7"/>
+      <c r="H60" s="7">
+        <v>0.76119999999999999</v>
+      </c>
       <c r="I60" s="7">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="6" t="e">
+        <v>8.6100000000000065E-2</v>
+      </c>
+      <c r="J60" s="7">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K60" s="6" t="e">
+        <v>0.89838309925646165</v>
+      </c>
+      <c r="K60" s="7">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>0.91380552220888356</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="10"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F61" s="11"/>
       <c r="G61" s="3">
         <v>2</v>
       </c>
-      <c r="H61" s="2"/>
+      <c r="H61" s="2">
+        <v>0.48060000000000003</v>
+      </c>
       <c r="I61" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="3" t="e">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="J61" s="2">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K61" s="3" t="e">
+        <v>0.56721350171131835</v>
+      </c>
+      <c r="K61" s="2">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>0.57695078031212488</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="11"/>
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F62" s="12"/>
       <c r="G62" s="3">
         <v>3</v>
       </c>
-      <c r="H62" s="2"/>
+      <c r="H62" s="2">
+        <v>0.1</v>
+      </c>
       <c r="I62" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="3" t="e">
+        <v>0.74730000000000008</v>
+      </c>
+      <c r="J62" s="2">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K62" s="3" t="e">
+        <v>0.11802195208308745</v>
+      </c>
+      <c r="K62" s="2">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>0.12004801920768308</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2444,349 +2498,433 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="12">
+      <c r="A64" s="13">
         <v>4</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B64" s="13">
         <v>2</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="13">
         <v>6</v>
       </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="12" t="s">
+      <c r="D64" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F64" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G64" s="3">
         <v>0</v>
       </c>
-      <c r="H64" s="2"/>
+      <c r="H64" s="2">
+        <v>0.91669999999999996</v>
+      </c>
       <c r="I64" s="2">
         <f>D64-H64</f>
-        <v>0</v>
-      </c>
-      <c r="J64" s="3" t="e">
+        <v>7.3400000000000021E-2</v>
+      </c>
+      <c r="J64" s="2">
         <f>H64/D64</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K64" s="3" t="e">
+        <v>0.92586607413392585</v>
+      </c>
+      <c r="K64" s="2">
         <f>H64/E64</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="12"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F65" s="13"/>
       <c r="G65" s="4">
         <v>1</v>
       </c>
-      <c r="H65" s="5"/>
+      <c r="H65" s="5">
+        <v>0.88380000000000003</v>
+      </c>
       <c r="I65" s="5">
         <f t="shared" ref="I65:I77" si="15">D65-H65</f>
-        <v>0</v>
-      </c>
-      <c r="J65" s="4" t="e">
+        <v>0.10629999999999995</v>
+      </c>
+      <c r="J65" s="5">
         <f t="shared" ref="J65:J77" si="16">H65/D65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K65" s="4" t="e">
+        <v>0.8926371073628927</v>
+      </c>
+      <c r="K65" s="5">
         <f t="shared" ref="K65:K77" si="17">H65/E65</f>
-        <v>#DIV/0!</v>
+        <v>0.96411039598560055</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="12"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F66" s="13"/>
       <c r="G66" s="4">
         <v>2</v>
       </c>
-      <c r="H66" s="5"/>
+      <c r="H66" s="5">
+        <v>0.83030000000000004</v>
+      </c>
       <c r="I66" s="5">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="4" t="e">
+        <v>0.15979999999999994</v>
+      </c>
+      <c r="J66" s="5">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K66" s="4" t="e">
+        <v>0.83860216139783861</v>
+      </c>
+      <c r="K66" s="5">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.90574888185884161</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="12"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F67" s="13"/>
       <c r="G67" s="3">
         <v>3</v>
       </c>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2">
+        <v>0.74709999999999999</v>
+      </c>
       <c r="I67" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J67" s="3" t="e">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="J67" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K67" s="3" t="e">
+        <v>0.75457024542975459</v>
+      </c>
+      <c r="K67" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.81498854587105929</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="12"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F68" s="13"/>
       <c r="G68" s="3">
         <v>4</v>
       </c>
-      <c r="H68" s="2"/>
+      <c r="H68" s="2">
+        <v>0.62470000000000003</v>
+      </c>
       <c r="I68" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J68" s="3" t="e">
+        <v>0.36539999999999995</v>
+      </c>
+      <c r="J68" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K68" s="3" t="e">
+        <v>0.630946369053631</v>
+      </c>
+      <c r="K68" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.68146612850441812</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="12"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F69" s="13"/>
       <c r="G69" s="3">
         <v>5</v>
       </c>
-      <c r="H69" s="2"/>
+      <c r="H69" s="2">
+        <v>0.40620000000000001</v>
+      </c>
       <c r="I69" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J69" s="3" t="e">
+        <v>0.58389999999999997</v>
+      </c>
+      <c r="J69" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K69" s="3" t="e">
+        <v>0.41026158973841026</v>
+      </c>
+      <c r="K69" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.44311115959419661</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="12"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="2">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="F70" s="13"/>
       <c r="G70" s="3">
         <v>6</v>
       </c>
-      <c r="H70" s="2"/>
+      <c r="H70" s="2">
+        <v>0.1</v>
+      </c>
       <c r="I70" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J70" s="3" t="e">
+        <v>0.8901</v>
+      </c>
+      <c r="J70" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K70" s="3" t="e">
+        <v>0.10099989900010101</v>
+      </c>
+      <c r="K70" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.10908694229300754</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="12" t="s">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F71" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G71" s="3">
         <v>0</v>
       </c>
-      <c r="H71" s="2"/>
+      <c r="H71" s="2">
+        <v>0.82269999999999999</v>
+      </c>
       <c r="I71" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J71" s="3" t="e">
+        <v>2.4600000000000066E-2</v>
+      </c>
+      <c r="J71" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K71" s="3" t="e">
+        <v>0.97096659978756039</v>
+      </c>
+      <c r="K71" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="12"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F72" s="13"/>
       <c r="G72" s="6">
         <v>1</v>
       </c>
-      <c r="H72" s="7"/>
+      <c r="H72" s="7">
+        <v>0.79400000000000004</v>
+      </c>
       <c r="I72" s="7">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J72" s="6" t="e">
+        <v>5.3300000000000014E-2</v>
+      </c>
+      <c r="J72" s="7">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K72" s="6" t="e">
+        <v>0.93709429953971435</v>
+      </c>
+      <c r="K72" s="7">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.96511486568615545</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="12"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F73" s="13"/>
       <c r="G73" s="6">
         <v>2</v>
       </c>
-      <c r="H73" s="7"/>
+      <c r="H73" s="7">
+        <v>0.752</v>
+      </c>
       <c r="I73" s="7">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J73" s="6" t="e">
+        <v>9.5300000000000051E-2</v>
+      </c>
+      <c r="J73" s="7">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K73" s="6" t="e">
+        <v>0.88752507966481764</v>
+      </c>
+      <c r="K73" s="7">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.91406344961711439</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="12"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F74" s="13"/>
       <c r="G74" s="3">
         <v>3</v>
       </c>
-      <c r="H74" s="2"/>
+      <c r="H74" s="2">
+        <v>0.68479999999999996</v>
+      </c>
       <c r="I74" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J74" s="3" t="e">
+        <v>0.16250000000000009</v>
+      </c>
+      <c r="J74" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K74" s="3" t="e">
+        <v>0.80821432786498282</v>
+      </c>
+      <c r="K74" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.83238118390664884</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="12"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F75" s="13"/>
       <c r="G75" s="3">
         <v>4</v>
       </c>
-      <c r="H75" s="2"/>
+      <c r="H75" s="2">
+        <v>0.60099999999999998</v>
+      </c>
       <c r="I75" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J75" s="3" t="e">
+        <v>0.24630000000000007</v>
+      </c>
+      <c r="J75" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K75" s="3" t="e">
+        <v>0.7093119320193555</v>
+      </c>
+      <c r="K75" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.730521453749848</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="12"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F76" s="13"/>
       <c r="G76" s="3">
         <v>5</v>
       </c>
-      <c r="H76" s="2"/>
+      <c r="H76" s="2">
+        <v>0.36320000000000002</v>
+      </c>
       <c r="I76" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J76" s="3" t="e">
+        <v>0.48410000000000003</v>
+      </c>
+      <c r="J76" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K76" s="3" t="e">
+        <v>0.42865572996577361</v>
+      </c>
+      <c r="K76" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.44147319800656376</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="12"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="2">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F77" s="13"/>
       <c r="G77" s="3">
         <v>6</v>
       </c>
-      <c r="H77" s="2"/>
+      <c r="H77" s="2">
+        <v>0.1</v>
+      </c>
       <c r="I77" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J77" s="3" t="e">
+        <v>0.74730000000000008</v>
+      </c>
+      <c r="J77" s="2">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K77" s="3" t="e">
+        <v>0.11802195208308745</v>
+      </c>
+      <c r="K77" s="2">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.12155099064057373</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -2803,19 +2941,19 @@
       <c r="K78" s="8"/>
     </row>
     <row r="79" spans="1:11" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2853,20 +2991,20 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+      <c r="A81" s="10">
         <v>2</v>
       </c>
-      <c r="B81" s="9">
-        <v>1</v>
-      </c>
-      <c r="C81" s="9">
+      <c r="B81" s="10">
+        <v>1</v>
+      </c>
+      <c r="C81" s="10">
         <v>3</v>
       </c>
       <c r="D81" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E81" s="2"/>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G81" s="3">
@@ -2887,14 +3025,14 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
       <c r="D82" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E82" s="2"/>
-      <c r="F82" s="10"/>
+      <c r="F82" s="11"/>
       <c r="G82" s="4">
         <v>1</v>
       </c>
@@ -2913,14 +3051,14 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
       <c r="D83" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E83" s="2"/>
-      <c r="F83" s="10"/>
+      <c r="F83" s="11"/>
       <c r="G83" s="3">
         <v>2</v>
       </c>
@@ -2939,14 +3077,14 @@
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
       <c r="D84" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E84" s="2"/>
-      <c r="F84" s="11"/>
+      <c r="F84" s="12"/>
       <c r="G84" s="3">
         <v>3</v>
       </c>
@@ -2965,14 +3103,14 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
       <c r="D85" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E85" s="2"/>
-      <c r="F85" s="9" t="s">
+      <c r="F85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G85" s="3">
@@ -2993,14 +3131,14 @@
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E86" s="2"/>
-      <c r="F86" s="10"/>
+      <c r="F86" s="11"/>
       <c r="G86" s="6">
         <v>1</v>
       </c>
@@ -3019,14 +3157,14 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
       <c r="D87" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E87" s="2"/>
-      <c r="F87" s="10"/>
+      <c r="F87" s="11"/>
       <c r="G87" s="3">
         <v>2</v>
       </c>
@@ -3045,14 +3183,14 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
       <c r="D88" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E88" s="2"/>
-      <c r="F88" s="11"/>
+      <c r="F88" s="12"/>
       <c r="G88" s="3">
         <v>3</v>
       </c>
@@ -3106,20 +3244,20 @@
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="12">
+      <c r="A90" s="13">
         <v>4</v>
       </c>
-      <c r="B90" s="12">
+      <c r="B90" s="13">
         <v>2</v>
       </c>
-      <c r="C90" s="12">
+      <c r="C90" s="13">
         <v>6</v>
       </c>
       <c r="D90" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E90" s="3"/>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G90" s="3">
@@ -3140,14 +3278,14 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
       <c r="D91" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E91" s="3"/>
-      <c r="F91" s="12"/>
+      <c r="F91" s="13"/>
       <c r="G91" s="4">
         <v>1</v>
       </c>
@@ -3166,14 +3304,14 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="12"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E92" s="3"/>
-      <c r="F92" s="12"/>
+      <c r="F92" s="13"/>
       <c r="G92" s="4">
         <v>2</v>
       </c>
@@ -3192,14 +3330,14 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E93" s="3"/>
-      <c r="F93" s="12"/>
+      <c r="F93" s="13"/>
       <c r="G93" s="3">
         <v>3</v>
       </c>
@@ -3218,14 +3356,14 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
       <c r="D94" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E94" s="3"/>
-      <c r="F94" s="12"/>
+      <c r="F94" s="13"/>
       <c r="G94" s="3">
         <v>4</v>
       </c>
@@ -3244,14 +3382,14 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
+      <c r="A95" s="13"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
       <c r="D95" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E95" s="3"/>
-      <c r="F95" s="12"/>
+      <c r="F95" s="13"/>
       <c r="G95" s="3">
         <v>5</v>
       </c>
@@ -3270,14 +3408,14 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="2">
         <v>0.99509999999999998</v>
       </c>
       <c r="E96" s="3"/>
-      <c r="F96" s="12"/>
+      <c r="F96" s="13"/>
       <c r="G96" s="3">
         <v>6</v>
       </c>
@@ -3296,14 +3434,14 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
+      <c r="A97" s="13"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
       <c r="D97" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E97" s="3"/>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G97" s="3">
@@ -3324,14 +3462,14 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
       <c r="D98" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E98" s="3"/>
-      <c r="F98" s="12"/>
+      <c r="F98" s="13"/>
       <c r="G98" s="6">
         <v>1</v>
       </c>
@@ -3350,14 +3488,14 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
+      <c r="A99" s="13"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
       <c r="D99" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E99" s="3"/>
-      <c r="F99" s="12"/>
+      <c r="F99" s="13"/>
       <c r="G99" s="6">
         <v>2</v>
       </c>
@@ -3376,14 +3514,14 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
-      <c r="C100" s="12"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
       <c r="D100" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E100" s="3"/>
-      <c r="F100" s="12"/>
+      <c r="F100" s="13"/>
       <c r="G100" s="3">
         <v>3</v>
       </c>
@@ -3402,14 +3540,14 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
       <c r="D101" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E101" s="3"/>
-      <c r="F101" s="12"/>
+      <c r="F101" s="13"/>
       <c r="G101" s="3">
         <v>4</v>
       </c>
@@ -3428,14 +3566,14 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
       <c r="D102" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E102" s="3"/>
-      <c r="F102" s="12"/>
+      <c r="F102" s="13"/>
       <c r="G102" s="3">
         <v>5</v>
       </c>
@@ -3454,14 +3592,14 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
-      <c r="C103" s="12"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
       <c r="D103" s="2">
         <v>0.98899999999999999</v>
       </c>
       <c r="E103" s="3"/>
-      <c r="F103" s="12"/>
+      <c r="F103" s="13"/>
       <c r="G103" s="3">
         <v>6</v>
       </c>
@@ -3480,19 +3618,19 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
@@ -3530,18 +3668,18 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="9">
+      <c r="A107" s="10">
         <v>2</v>
       </c>
-      <c r="B107" s="9">
-        <v>1</v>
-      </c>
-      <c r="C107" s="9">
+      <c r="B107" s="10">
+        <v>1</v>
+      </c>
+      <c r="C107" s="10">
         <v>3</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
-      <c r="F107" s="9" t="s">
+      <c r="F107" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G107" s="3">
@@ -3562,12 +3700,12 @@
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10"/>
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="F108" s="10"/>
+      <c r="F108" s="11"/>
       <c r="G108" s="4">
         <v>1</v>
       </c>
@@ -3586,12 +3724,12 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10"/>
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
-      <c r="F109" s="10"/>
+      <c r="F109" s="11"/>
       <c r="G109" s="3">
         <v>2</v>
       </c>
@@ -3610,12 +3748,12 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="10"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
-      <c r="F110" s="11"/>
+      <c r="F110" s="12"/>
       <c r="G110" s="3">
         <v>3</v>
       </c>
@@ -3634,12 +3772,12 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="11"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
-      <c r="F111" s="9" t="s">
+      <c r="F111" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G111" s="3">
@@ -3660,12 +3798,12 @@
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
-      <c r="F112" s="10"/>
+      <c r="F112" s="11"/>
       <c r="G112" s="6">
         <v>1</v>
       </c>
@@ -3684,12 +3822,12 @@
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
-      <c r="F113" s="10"/>
+      <c r="F113" s="11"/>
       <c r="G113" s="3">
         <v>2</v>
       </c>
@@ -3708,12 +3846,12 @@
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
-      <c r="F114" s="11"/>
+      <c r="F114" s="12"/>
       <c r="G114" s="3">
         <v>3</v>
       </c>
@@ -3767,18 +3905,18 @@
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="12">
+      <c r="A116" s="13">
         <v>4</v>
       </c>
-      <c r="B116" s="12">
+      <c r="B116" s="13">
         <v>2</v>
       </c>
-      <c r="C116" s="12">
+      <c r="C116" s="13">
         <v>6</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="12" t="s">
+      <c r="F116" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G116" s="3">
@@ -3799,12 +3937,12 @@
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="12"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="13"/>
       <c r="D117" s="2"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="12"/>
+      <c r="F117" s="13"/>
       <c r="G117" s="4">
         <v>1</v>
       </c>
@@ -3823,12 +3961,12 @@
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
-      <c r="C118" s="12"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="13"/>
       <c r="D118" s="2"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="12"/>
+      <c r="F118" s="13"/>
       <c r="G118" s="4">
         <v>2</v>
       </c>
@@ -3847,12 +3985,12 @@
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
       <c r="D119" s="2"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="12"/>
+      <c r="F119" s="13"/>
       <c r="G119" s="3">
         <v>3</v>
       </c>
@@ -3871,12 +4009,12 @@
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="12"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="13"/>
       <c r="D120" s="2"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="12"/>
+      <c r="F120" s="13"/>
       <c r="G120" s="3">
         <v>4</v>
       </c>
@@ -3895,12 +4033,12 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
       <c r="D121" s="2"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="12"/>
+      <c r="F121" s="13"/>
       <c r="G121" s="3">
         <v>5</v>
       </c>
@@ -3919,12 +4057,12 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="C122" s="12"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
       <c r="D122" s="2"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="12"/>
+      <c r="F122" s="13"/>
       <c r="G122" s="3">
         <v>6</v>
       </c>
@@ -3943,12 +4081,12 @@
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
       <c r="D123" s="2"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="12" t="s">
+      <c r="F123" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G123" s="3">
@@ -3969,12 +4107,12 @@
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
       <c r="D124" s="2"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="12"/>
+      <c r="F124" s="13"/>
       <c r="G124" s="6">
         <v>1</v>
       </c>
@@ -3993,12 +4131,12 @@
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
       <c r="D125" s="2"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="12"/>
+      <c r="F125" s="13"/>
       <c r="G125" s="6">
         <v>2</v>
       </c>
@@ -4017,12 +4155,12 @@
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
-      <c r="B126" s="12"/>
-      <c r="C126" s="12"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
       <c r="D126" s="2"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="12"/>
+      <c r="F126" s="13"/>
       <c r="G126" s="3">
         <v>3</v>
       </c>
@@ -4041,12 +4179,12 @@
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="12"/>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
       <c r="D127" s="2"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="12"/>
+      <c r="F127" s="13"/>
       <c r="G127" s="3">
         <v>4</v>
       </c>
@@ -4065,12 +4203,12 @@
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="12"/>
-      <c r="B128" s="12"/>
-      <c r="C128" s="12"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
       <c r="D128" s="2"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="12"/>
+      <c r="F128" s="13"/>
       <c r="G128" s="3">
         <v>5</v>
       </c>
@@ -4089,12 +4227,12 @@
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
       <c r="D129" s="2"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="12"/>
+      <c r="F129" s="13"/>
       <c r="G129" s="3">
         <v>6</v>
       </c>
@@ -4113,19 +4251,19 @@
       </c>
     </row>
     <row r="131" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="13" t="s">
+      <c r="A131" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B131" s="13"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
@@ -4163,18 +4301,18 @@
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="9">
+      <c r="A133" s="10">
         <v>2</v>
       </c>
-      <c r="B133" s="9">
-        <v>1</v>
-      </c>
-      <c r="C133" s="9">
+      <c r="B133" s="10">
+        <v>1</v>
+      </c>
+      <c r="C133" s="10">
         <v>3</v>
       </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
-      <c r="F133" s="9" t="s">
+      <c r="F133" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G133" s="3">
@@ -4195,12 +4333,12 @@
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="10"/>
-      <c r="B134" s="10"/>
-      <c r="C134" s="10"/>
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
-      <c r="F134" s="10"/>
+      <c r="F134" s="11"/>
       <c r="G134" s="4">
         <v>1</v>
       </c>
@@ -4219,12 +4357,12 @@
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="10"/>
-      <c r="B135" s="10"/>
-      <c r="C135" s="10"/>
+      <c r="A135" s="11"/>
+      <c r="B135" s="11"/>
+      <c r="C135" s="11"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
-      <c r="F135" s="10"/>
+      <c r="F135" s="11"/>
       <c r="G135" s="3">
         <v>2</v>
       </c>
@@ -4243,12 +4381,12 @@
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="10"/>
-      <c r="B136" s="10"/>
-      <c r="C136" s="10"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="11"/>
+      <c r="C136" s="11"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
-      <c r="F136" s="11"/>
+      <c r="F136" s="12"/>
       <c r="G136" s="3">
         <v>3</v>
       </c>
@@ -4267,12 +4405,12 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
-      <c r="B137" s="10"/>
-      <c r="C137" s="10"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
+      <c r="C137" s="11"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="F137" s="9" t="s">
+      <c r="F137" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G137" s="3">
@@ -4293,12 +4431,12 @@
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="10"/>
-      <c r="B138" s="10"/>
-      <c r="C138" s="10"/>
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
+      <c r="C138" s="11"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
-      <c r="F138" s="10"/>
+      <c r="F138" s="11"/>
       <c r="G138" s="6">
         <v>1</v>
       </c>
@@ -4317,12 +4455,12 @@
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="10"/>
-      <c r="B139" s="10"/>
-      <c r="C139" s="10"/>
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
+      <c r="C139" s="11"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
-      <c r="F139" s="10"/>
+      <c r="F139" s="11"/>
       <c r="G139" s="3">
         <v>2</v>
       </c>
@@ -4341,12 +4479,12 @@
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
+      <c r="A140" s="12"/>
+      <c r="B140" s="12"/>
+      <c r="C140" s="12"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
-      <c r="F140" s="11"/>
+      <c r="F140" s="12"/>
       <c r="G140" s="3">
         <v>3</v>
       </c>
@@ -4400,18 +4538,18 @@
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="12">
+      <c r="A142" s="13">
         <v>4</v>
       </c>
-      <c r="B142" s="12">
+      <c r="B142" s="13">
         <v>2</v>
       </c>
-      <c r="C142" s="12">
+      <c r="C142" s="13">
         <v>6</v>
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="12" t="s">
+      <c r="F142" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G142" s="3">
@@ -4432,12 +4570,12 @@
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="12"/>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
       <c r="D143" s="2"/>
       <c r="E143" s="3"/>
-      <c r="F143" s="12"/>
+      <c r="F143" s="13"/>
       <c r="G143" s="4">
         <v>1</v>
       </c>
@@ -4456,12 +4594,12 @@
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144" s="12"/>
-      <c r="B144" s="12"/>
-      <c r="C144" s="12"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
       <c r="D144" s="2"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="12"/>
+      <c r="F144" s="13"/>
       <c r="G144" s="4">
         <v>2</v>
       </c>
@@ -4480,12 +4618,12 @@
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="12"/>
-      <c r="B145" s="12"/>
-      <c r="C145" s="12"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
       <c r="D145" s="2"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="12"/>
+      <c r="F145" s="13"/>
       <c r="G145" s="3">
         <v>3</v>
       </c>
@@ -4504,12 +4642,12 @@
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="12"/>
-      <c r="B146" s="12"/>
-      <c r="C146" s="12"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="13"/>
       <c r="D146" s="2"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="12"/>
+      <c r="F146" s="13"/>
       <c r="G146" s="3">
         <v>4</v>
       </c>
@@ -4528,12 +4666,12 @@
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
-      <c r="B147" s="12"/>
-      <c r="C147" s="12"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
       <c r="D147" s="2"/>
       <c r="E147" s="3"/>
-      <c r="F147" s="12"/>
+      <c r="F147" s="13"/>
       <c r="G147" s="3">
         <v>5</v>
       </c>
@@ -4552,12 +4690,12 @@
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148" s="12"/>
-      <c r="B148" s="12"/>
-      <c r="C148" s="12"/>
+      <c r="A148" s="13"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
       <c r="D148" s="2"/>
       <c r="E148" s="3"/>
-      <c r="F148" s="12"/>
+      <c r="F148" s="13"/>
       <c r="G148" s="3">
         <v>6</v>
       </c>
@@ -4576,12 +4714,12 @@
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149" s="12"/>
-      <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
+      <c r="A149" s="13"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
       <c r="D149" s="2"/>
       <c r="E149" s="3"/>
-      <c r="F149" s="12" t="s">
+      <c r="F149" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G149" s="3">
@@ -4602,12 +4740,12 @@
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150" s="12"/>
-      <c r="B150" s="12"/>
-      <c r="C150" s="12"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="13"/>
+      <c r="C150" s="13"/>
       <c r="D150" s="2"/>
       <c r="E150" s="3"/>
-      <c r="F150" s="12"/>
+      <c r="F150" s="13"/>
       <c r="G150" s="6">
         <v>1</v>
       </c>
@@ -4626,12 +4764,12 @@
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151" s="12"/>
-      <c r="B151" s="12"/>
-      <c r="C151" s="12"/>
+      <c r="A151" s="13"/>
+      <c r="B151" s="13"/>
+      <c r="C151" s="13"/>
       <c r="D151" s="2"/>
       <c r="E151" s="3"/>
-      <c r="F151" s="12"/>
+      <c r="F151" s="13"/>
       <c r="G151" s="6">
         <v>2</v>
       </c>
@@ -4650,12 +4788,12 @@
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A152" s="12"/>
-      <c r="B152" s="12"/>
-      <c r="C152" s="12"/>
+      <c r="A152" s="13"/>
+      <c r="B152" s="13"/>
+      <c r="C152" s="13"/>
       <c r="D152" s="2"/>
       <c r="E152" s="3"/>
-      <c r="F152" s="12"/>
+      <c r="F152" s="13"/>
       <c r="G152" s="3">
         <v>3</v>
       </c>
@@ -4674,12 +4812,12 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153" s="12"/>
-      <c r="B153" s="12"/>
-      <c r="C153" s="12"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="13"/>
+      <c r="C153" s="13"/>
       <c r="D153" s="2"/>
       <c r="E153" s="3"/>
-      <c r="F153" s="12"/>
+      <c r="F153" s="13"/>
       <c r="G153" s="3">
         <v>4</v>
       </c>
@@ -4698,12 +4836,12 @@
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154" s="12"/>
-      <c r="B154" s="12"/>
-      <c r="C154" s="12"/>
+      <c r="A154" s="13"/>
+      <c r="B154" s="13"/>
+      <c r="C154" s="13"/>
       <c r="D154" s="2"/>
       <c r="E154" s="3"/>
-      <c r="F154" s="12"/>
+      <c r="F154" s="13"/>
       <c r="G154" s="3">
         <v>5</v>
       </c>
@@ -4722,12 +4860,12 @@
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A155" s="12"/>
-      <c r="B155" s="12"/>
-      <c r="C155" s="12"/>
+      <c r="A155" s="13"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
       <c r="D155" s="2"/>
       <c r="E155" s="3"/>
-      <c r="F155" s="12"/>
+      <c r="F155" s="13"/>
       <c r="G155" s="3">
         <v>6</v>
       </c>
@@ -4747,6 +4885,60 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A133:A140"/>
+    <mergeCell ref="B133:B140"/>
+    <mergeCell ref="C133:C140"/>
+    <mergeCell ref="F133:F136"/>
+    <mergeCell ref="F137:F140"/>
+    <mergeCell ref="A142:A155"/>
+    <mergeCell ref="B142:B155"/>
+    <mergeCell ref="C142:C155"/>
+    <mergeCell ref="F142:F148"/>
+    <mergeCell ref="F149:F155"/>
+    <mergeCell ref="A131:K131"/>
+    <mergeCell ref="A105:K105"/>
+    <mergeCell ref="A107:A114"/>
+    <mergeCell ref="B107:B114"/>
+    <mergeCell ref="C107:C114"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="A116:A129"/>
+    <mergeCell ref="B116:B129"/>
+    <mergeCell ref="C116:C129"/>
+    <mergeCell ref="F116:F122"/>
+    <mergeCell ref="F123:F129"/>
+    <mergeCell ref="A81:A88"/>
+    <mergeCell ref="B81:B88"/>
+    <mergeCell ref="C81:C88"/>
+    <mergeCell ref="F81:F84"/>
+    <mergeCell ref="F85:F88"/>
+    <mergeCell ref="A90:A103"/>
+    <mergeCell ref="B90:B103"/>
+    <mergeCell ref="C90:C103"/>
+    <mergeCell ref="F90:F96"/>
+    <mergeCell ref="F97:F103"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="A64:A77"/>
+    <mergeCell ref="B64:B77"/>
+    <mergeCell ref="C64:C77"/>
+    <mergeCell ref="F64:F70"/>
+    <mergeCell ref="F71:F77"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="A38:A51"/>
+    <mergeCell ref="B38:B51"/>
+    <mergeCell ref="C38:C51"/>
+    <mergeCell ref="F38:F44"/>
+    <mergeCell ref="F45:F51"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:A10"/>
@@ -4759,60 +4951,6 @@
     <mergeCell ref="C12:C25"/>
     <mergeCell ref="F12:F18"/>
     <mergeCell ref="F19:F25"/>
-    <mergeCell ref="A38:A51"/>
-    <mergeCell ref="B38:B51"/>
-    <mergeCell ref="C38:C51"/>
-    <mergeCell ref="F38:F44"/>
-    <mergeCell ref="F45:F51"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="B55:B62"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="F59:F62"/>
-    <mergeCell ref="A64:A77"/>
-    <mergeCell ref="B64:B77"/>
-    <mergeCell ref="C64:C77"/>
-    <mergeCell ref="F64:F70"/>
-    <mergeCell ref="F71:F77"/>
-    <mergeCell ref="A90:A103"/>
-    <mergeCell ref="B90:B103"/>
-    <mergeCell ref="C90:C103"/>
-    <mergeCell ref="F90:F96"/>
-    <mergeCell ref="F97:F103"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="B81:B88"/>
-    <mergeCell ref="C81:C88"/>
-    <mergeCell ref="F81:F84"/>
-    <mergeCell ref="F85:F88"/>
-    <mergeCell ref="A131:K131"/>
-    <mergeCell ref="A105:K105"/>
-    <mergeCell ref="A107:A114"/>
-    <mergeCell ref="B107:B114"/>
-    <mergeCell ref="C107:C114"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="F111:F114"/>
-    <mergeCell ref="A116:A129"/>
-    <mergeCell ref="B116:B129"/>
-    <mergeCell ref="C116:C129"/>
-    <mergeCell ref="F116:F122"/>
-    <mergeCell ref="F123:F129"/>
-    <mergeCell ref="A142:A155"/>
-    <mergeCell ref="B142:B155"/>
-    <mergeCell ref="C142:C155"/>
-    <mergeCell ref="F142:F148"/>
-    <mergeCell ref="F149:F155"/>
-    <mergeCell ref="A133:A140"/>
-    <mergeCell ref="B133:B140"/>
-    <mergeCell ref="C133:C140"/>
-    <mergeCell ref="F133:F136"/>
-    <mergeCell ref="F137:F140"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>